<commit_message>
Completando la tercera parte
</commit_message>
<xml_diff>
--- a/PARTE MARVIN(3ra_parte)/proteina4.xlsx
+++ b/PARTE MARVIN(3ra_parte)/proteina4.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb48aa08db57dad8/Escritorio/Trabajo final/TRABAJO-FINAL-GRUPO-D/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_FFC65FC073016BD184160B1D5348F35567C4DE6F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -313,8 +319,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,11 +383,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,7 +437,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,9 +469,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,6 +521,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -664,19 +714,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -684,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -692,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -700,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -708,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -716,7 +768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -724,7 +776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -732,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -740,7 +792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -748,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -756,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -764,7 +816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -772,7 +824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -780,7 +832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -788,7 +840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -796,7 +848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -804,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -812,7 +864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -820,7 +872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -828,7 +880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -836,7 +888,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -844,7 +896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -852,7 +904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -860,7 +912,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -868,7 +920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -876,7 +928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -884,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -892,7 +944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -900,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -908,7 +960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -916,7 +968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -924,7 +976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -932,7 +984,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -940,7 +992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -948,7 +1000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -956,7 +1008,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -964,7 +1016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -972,7 +1024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -980,7 +1032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -988,7 +1040,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -996,7 +1048,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1004,7 +1056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1012,7 +1064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1020,7 +1072,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1028,7 +1080,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1036,7 +1088,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1044,7 +1096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1052,7 +1104,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1060,7 +1112,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1068,7 +1120,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1076,7 +1128,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1084,7 +1136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1092,7 +1144,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1100,7 +1152,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1108,7 +1160,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1116,7 +1168,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1124,7 +1176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1132,7 +1184,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1140,7 +1192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1148,7 +1200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1156,7 +1208,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1164,7 +1216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1172,7 +1224,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1180,7 +1232,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1188,7 +1240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1196,7 +1248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1204,7 +1256,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1212,7 +1264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1220,7 +1272,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1228,7 +1280,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1236,7 +1288,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1244,7 +1296,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1252,7 +1304,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1260,7 +1312,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1268,7 +1320,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1276,7 +1328,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1284,7 +1336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1292,7 +1344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1300,7 +1352,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1308,7 +1360,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1316,7 +1368,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1324,7 +1376,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1332,7 +1384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1340,7 +1392,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1348,7 +1400,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1356,7 +1408,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1364,7 +1416,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1372,7 +1424,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1380,7 +1432,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1388,7 +1440,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1396,7 +1448,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1404,7 +1456,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1412,7 +1464,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1420,7 +1472,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1428,7 +1480,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -1436,7 +1488,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -1444,7 +1496,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1452,7 +1504,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1460,7 +1512,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1468,7 +1520,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>

</xml_diff>